<commit_message>
Forgot to use FastPossible when running the simulations.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestProjects/PerformanceTests/Performace.xlsx
+++ b/Libraries/AnimatTesting/TestProjects/PerformanceTests/Performace.xlsx
@@ -453,11 +453,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="123881344"/>
-        <c:axId val="123882880"/>
+        <c:axId val="123885440"/>
+        <c:axId val="123886976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="123881344"/>
+        <c:axId val="123885440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +467,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123882880"/>
+        <c:crossAx val="123886976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -475,7 +475,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123882880"/>
+        <c:axId val="123886976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123881344"/>
+        <c:crossAx val="123885440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -561,7 +561,7 @@
                   <c:v>2.9836999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8222019999999998E-4</c:v>
+                  <c:v>2.77543E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,7 +2079,7 @@
         <v>3.0439200000000001E-4</v>
       </c>
       <c r="B2">
-        <v>2.8765099999999999E-4</v>
+        <v>2.8185500000000002E-4</v>
       </c>
       <c r="E2">
         <f>AVERAGE(A2:A6)</f>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="F2">
         <f>AVERAGE(B2:B6)</f>
-        <v>2.8222019999999998E-4</v>
+        <v>2.77543E-4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
         <v>2.9393600000000001E-4</v>
       </c>
       <c r="B3">
-        <v>2.79919E-4</v>
+        <v>2.6560400000000001E-4</v>
       </c>
       <c r="E3">
         <f>_xlfn.STDEV.P(A2:A6)</f>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="F3">
         <f>_xlfn.STDEV.P(B2:B6)</f>
-        <v>7.1876589624160743E-6</v>
+        <v>9.2475202730245505E-6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2119,7 +2119,7 @@
         <v>3.0115099999999999E-4</v>
       </c>
       <c r="B5">
-        <v>2.8492200000000001E-4</v>
+        <v>2.9152200000000001E-4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,7 +2127,7 @@
         <v>2.9863699999999998E-4</v>
       </c>
       <c r="B6">
-        <v>2.8928500000000002E-4</v>
+        <v>2.7941000000000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>